<commit_message>
Updated graph and excel files
</commit_message>
<xml_diff>
--- a/Sensor Box Version 2/distance_calibrating.xlsx
+++ b/Sensor Box Version 2/distance_calibrating.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Noahv\OneDrive\Documenten\School\Design_n_contruction\Wing Design\Sensors\Sensor Box Version 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E33A70E1-8EA4-4590-8033-93AAA161593C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CCBAE73-E398-4EA8-A1A8-29D5FAF1395B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -97,6 +97,21 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="nl-NL"/>
+              <a:t>Distance calibration</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -121,6 +136,12 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.22217756905015953"/>
+                  <c:y val="0.2568864186094385"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -197,6 +218,24 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nl-NL"/>
+                  <a:t>Real distance (mm)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -213,6 +252,28 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nl-NL"/>
+                  <a:t>Measured</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="nl-NL" baseline="0"/>
+                  <a:t> distance (mm)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -242,16 +303,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>276224</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -603,7 +664,7 @@
   <dimension ref="A1:V61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="A4:B5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>